<commit_message>
Added Edit and verification method
</commit_message>
<xml_diff>
--- a/LearnSmartAutomation/TestCaseData.xlsx
+++ b/LearnSmartAutomation/TestCaseData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse-21\Workspace\NewLearnSmart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\LearnSmartAutomation\LearnSmartAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDD7264-C6DF-448C-88DA-CED4D2C0DF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A6B9E1-F823-40F2-AC87-31D8E513AFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="DemoTestCaseSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DemoTestCaseSheet!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DemoTestCaseSheet!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Sr.No</t>
   </si>
@@ -107,13 +107,37 @@
   </si>
   <si>
     <t>quizzesFlag</t>
+  </si>
+  <si>
+    <t>createNewFlag</t>
+  </si>
+  <si>
+    <t>editFlag</t>
+  </si>
+  <si>
+    <t>testCase_2</t>
+  </si>
+  <si>
+    <t>Second TC</t>
+  </si>
+  <si>
+    <t>editCourseName</t>
+  </si>
+  <si>
+    <t>Test Auto</t>
+  </si>
+  <si>
+    <t>Edited Course</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,12 +151,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -176,20 +194,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q7" sqref="Q7"/>
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,20 +492,22 @@
     <col min="1" max="1" width="12.6640625" style="2"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.6640625" style="2"/>
-    <col min="5" max="8" width="12.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" style="2" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" style="2"/>
-    <col min="12" max="12" width="13.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" style="2"/>
-    <col min="16" max="16" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="12.6640625" style="2"/>
+    <col min="14" max="14" width="13.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" style="2"/>
-    <col min="18" max="18" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="12.6640625" style="2"/>
+    <col min="18" max="18" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="2"/>
+    <col min="20" max="20" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,38 +530,46 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="1"/>
+      <c r="T1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -567,35 +591,89 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="2">
-        <v>1</v>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="T3" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>